<commit_message>
Remove all LFS-tracked files and add them as regular Git files
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33511</v>
+        <v>3038</v>
       </c>
       <c r="C2" t="n">
-        <v>523.1343439467637</v>
+        <v>476.0121790651745</v>
       </c>
       <c r="D2" t="n">
-        <v>85.68662258410087</v>
+        <v>50.37639214489838</v>
       </c>
       <c r="E2" t="n">
-        <v>392</v>
+        <v>407</v>
       </c>
       <c r="F2" t="n">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="G2" t="n">
+        <v>453</v>
+      </c>
+      <c r="H2" t="n">
         <v>512</v>
       </c>
-      <c r="H2" t="n">
-        <v>555</v>
-      </c>
       <c r="I2" t="n">
-        <v>1168</v>
+        <v>672</v>
       </c>
     </row>
     <row r="3">
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C3" t="n">
-        <v>58.13628677195697</v>
+        <v>57.26076491399292</v>
       </c>
       <c r="D3" t="n">
-        <v>6.57711436821135</v>
+        <v>6.131069641327043</v>
       </c>
       <c r="E3" t="n">
-        <v>38.26</v>
+        <v>43.05</v>
       </c>
       <c r="F3" t="n">
-        <v>53.86</v>
+        <v>53.13</v>
       </c>
       <c r="G3" t="n">
-        <v>59.27</v>
+        <v>57.48</v>
       </c>
       <c r="H3" t="n">
-        <v>63</v>
+        <v>60.87</v>
       </c>
       <c r="I3" t="n">
-        <v>76.5</v>
+        <v>77.73</v>
       </c>
     </row>
     <row r="4">
@@ -544,28 +544,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33511</v>
+        <v>8197</v>
       </c>
       <c r="C4" t="n">
-        <v>9.679920623078988</v>
+        <v>11.10812736366964</v>
       </c>
       <c r="D4" t="n">
-        <v>10.34629240669687</v>
+        <v>14.77310032576502</v>
       </c>
       <c r="E4" t="n">
-        <v>0.83</v>
+        <v>0.85</v>
       </c>
       <c r="F4" t="n">
-        <v>4.69</v>
+        <v>7.26</v>
       </c>
       <c r="G4" t="n">
-        <v>8.140000000000001</v>
+        <v>11.82</v>
       </c>
       <c r="H4" t="n">
-        <v>11.61</v>
+        <v>13.44</v>
       </c>
       <c r="I4" t="n">
-        <v>310.39</v>
+        <v>402.27</v>
       </c>
     </row>
     <row r="5">
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>33511</v>
+        <v>8197</v>
       </c>
       <c r="C5" t="n">
-        <v>328.0880648145385</v>
+        <v>323.2362742466756</v>
       </c>
       <c r="D5" t="n">
-        <v>3.895490435070943</v>
+        <v>1.951333985013952</v>
       </c>
       <c r="E5" t="n">
-        <v>317.47</v>
+        <v>319.47</v>
       </c>
       <c r="F5" t="n">
-        <v>325.11</v>
+        <v>321.45</v>
       </c>
       <c r="G5" t="n">
-        <v>328.25</v>
+        <v>323.5</v>
       </c>
       <c r="H5" t="n">
-        <v>331.01</v>
+        <v>324.94</v>
       </c>
       <c r="I5" t="n">
-        <v>335.53</v>
+        <v>326.61</v>
       </c>
     </row>
     <row r="6">
@@ -606,28 +606,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C6" t="n">
-        <v>23.29909957064616</v>
+        <v>26.0875613029157</v>
       </c>
       <c r="D6" t="n">
-        <v>1.853533996499332</v>
+        <v>1.650431260855432</v>
       </c>
       <c r="E6" t="n">
-        <v>18.62</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>22.2</v>
+        <v>25.48</v>
       </c>
       <c r="G6" t="n">
-        <v>23.3</v>
+        <v>26.35</v>
       </c>
       <c r="H6" t="n">
-        <v>24.65</v>
+        <v>27.19</v>
       </c>
       <c r="I6" t="n">
-        <v>28.83</v>
+        <v>29.99</v>
       </c>
     </row>
     <row r="7">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C7" t="n">
-        <v>-46.84792074401104</v>
+        <v>-46.58728803220691</v>
       </c>
       <c r="D7" t="n">
-        <v>13.48993094889533</v>
+        <v>10.20621201600229</v>
       </c>
       <c r="E7" t="n">
-        <v>-126</v>
+        <v>-128</v>
       </c>
       <c r="F7" t="n">
-        <v>-58</v>
+        <v>-57</v>
       </c>
       <c r="G7" t="n">
-        <v>-50</v>
+        <v>-43</v>
       </c>
       <c r="H7" t="n">
-        <v>-34</v>
+        <v>-38</v>
       </c>
       <c r="I7" t="n">
-        <v>-26</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="8">
@@ -668,28 +668,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>65913</v>
+        <v>8196</v>
       </c>
       <c r="C8" t="n">
-        <v>10.38297604417945</v>
+        <v>10.26993655441679</v>
       </c>
       <c r="D8" t="n">
-        <v>2.308493907888181</v>
+        <v>1.771792829661422</v>
       </c>
       <c r="E8" t="n">
-        <v>-21.5</v>
+        <v>-23.5</v>
       </c>
       <c r="F8" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="G8" t="n">
-        <v>10.5</v>
+        <v>10.2</v>
       </c>
       <c r="H8" t="n">
         <v>11.8</v>
       </c>
       <c r="I8" t="n">
-        <v>14.8</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="9">
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C9" t="n">
-        <v>8.89445177734286</v>
+        <v>9.386726851287056</v>
       </c>
       <c r="D9" t="n">
-        <v>1.381658485573381</v>
+        <v>1.676426131130018</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -717,10 +717,10 @@
         <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I9" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8212446710056</v>
+        <v>867.8380261071123</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4596133189424726</v>
+        <v>0.46382526644809</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,28 +761,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>65913</v>
+        <v>8196</v>
       </c>
       <c r="C11" t="n">
-        <v>13105.44092971038</v>
+        <v>1632.619204489995</v>
       </c>
       <c r="D11" t="n">
-        <v>8020.614775637623</v>
+        <v>1050.750478570848</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>6571</v>
+        <v>757</v>
       </c>
       <c r="G11" t="n">
-        <v>12266</v>
+        <v>1474.5</v>
       </c>
       <c r="H11" t="n">
-        <v>19388</v>
+        <v>2487.25</v>
       </c>
       <c r="I11" t="n">
-        <v>29021</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="12">
@@ -792,28 +792,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C12" t="n">
-        <v>14159.71529136893</v>
+        <v>1743.127729657192</v>
       </c>
       <c r="D12" t="n">
-        <v>8856.343186195863</v>
+        <v>1129.67439147521</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>6983</v>
+        <v>801</v>
       </c>
       <c r="G12" t="n">
-        <v>13002</v>
+        <v>1576</v>
       </c>
       <c r="H12" t="n">
-        <v>21313</v>
+        <v>2641</v>
       </c>
       <c r="I12" t="n">
-        <v>31936</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="13">
@@ -823,28 +823,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C13" t="n">
-        <v>0.323967497033969</v>
+        <v>0.525505163352446</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2889974046419547</v>
+        <v>0.5409177378327277</v>
       </c>
       <c r="E13" t="n">
         <v>0.061696</v>
       </c>
       <c r="F13" t="n">
-        <v>0.113152</v>
+        <v>0.123392</v>
       </c>
       <c r="G13" t="n">
-        <v>0.205824</v>
+        <v>0.246784</v>
       </c>
       <c r="H13" t="n">
-        <v>0.452608</v>
+        <v>0.823296</v>
       </c>
       <c r="I13" t="n">
-        <v>0.987136</v>
+        <v>1.974272</v>
       </c>
     </row>
     <row r="14">
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04542063022469014</v>
+        <v>0.04610345248261561</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02499665077304046</v>
+        <v>0.02173463530691788</v>
       </c>
       <c r="E14" t="n">
         <v>0.02</v>
@@ -869,7 +869,7 @@
         <v>0.02</v>
       </c>
       <c r="G14" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="H14" t="n">
         <v>0.07000000000000001</v>
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -947,13 +947,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4</v>
+        <v>0.4000000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>3.912455617829144e-13</v>
+        <v>5.745754642241973e-14</v>
       </c>
       <c r="E17" t="n">
         <v>0.4</v>
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C18" t="n">
         <v>3</v>
@@ -1009,28 +1009,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>65913</v>
+        <v>8197</v>
       </c>
       <c r="C19" t="n">
-        <v>63.24792074401103</v>
+        <v>62.9872880322069</v>
       </c>
       <c r="D19" t="n">
-        <v>13.48993094889616</v>
+        <v>10.20621201600226</v>
       </c>
       <c r="E19" t="n">
-        <v>42.4</v>
+        <v>44.4</v>
       </c>
       <c r="F19" t="n">
-        <v>50.4</v>
+        <v>54.4</v>
       </c>
       <c r="G19" t="n">
-        <v>66.40000000000001</v>
+        <v>59.4</v>
       </c>
       <c r="H19" t="n">
-        <v>74.40000000000001</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="I19" t="n">
-        <v>142.4</v>
+        <v>144.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit with more data!
</commit_message>
<xml_diff>
--- a/statistical_description.xlsx
+++ b/statistical_description.xlsx
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3038</v>
+        <v>3106</v>
       </c>
       <c r="C2" t="n">
-        <v>476.0121790651745</v>
+        <v>477.1687057308436</v>
       </c>
       <c r="D2" t="n">
-        <v>50.37639214489838</v>
+        <v>50.46616697433213</v>
       </c>
       <c r="E2" t="n">
         <v>407</v>
@@ -497,10 +497,10 @@
         <v>441</v>
       </c>
       <c r="G2" t="n">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H2" t="n">
-        <v>512</v>
+        <v>515.75</v>
       </c>
       <c r="I2" t="n">
         <v>672</v>
@@ -513,25 +513,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C3" t="n">
-        <v>57.26076491399292</v>
+        <v>57.34298500357058</v>
       </c>
       <c r="D3" t="n">
-        <v>6.131069641327043</v>
+        <v>6.177880403290533</v>
       </c>
       <c r="E3" t="n">
         <v>43.05</v>
       </c>
       <c r="F3" t="n">
-        <v>53.13</v>
+        <v>53.23</v>
       </c>
       <c r="G3" t="n">
-        <v>57.48</v>
+        <v>57.51</v>
       </c>
       <c r="H3" t="n">
-        <v>60.87</v>
+        <v>60.88</v>
       </c>
       <c r="I3" t="n">
         <v>77.73</v>
@@ -544,25 +544,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C4" t="n">
-        <v>11.10812736366964</v>
+        <v>11.28194715543918</v>
       </c>
       <c r="D4" t="n">
-        <v>14.77310032576502</v>
+        <v>15.89387772366126</v>
       </c>
       <c r="E4" t="n">
         <v>0.85</v>
       </c>
       <c r="F4" t="n">
-        <v>7.26</v>
+        <v>6.73</v>
       </c>
       <c r="G4" t="n">
-        <v>11.82</v>
+        <v>11.74</v>
       </c>
       <c r="H4" t="n">
-        <v>13.44</v>
+        <v>13.42</v>
       </c>
       <c r="I4" t="n">
         <v>402.27</v>
@@ -575,25 +575,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C5" t="n">
-        <v>323.2362742466756</v>
+        <v>323.2435800999762</v>
       </c>
       <c r="D5" t="n">
-        <v>1.951333985013952</v>
+        <v>1.929981559305362</v>
       </c>
       <c r="E5" t="n">
         <v>319.47</v>
       </c>
       <c r="F5" t="n">
-        <v>321.45</v>
+        <v>321.5625</v>
       </c>
       <c r="G5" t="n">
-        <v>323.5</v>
+        <v>323.52</v>
       </c>
       <c r="H5" t="n">
-        <v>324.94</v>
+        <v>324.89</v>
       </c>
       <c r="I5" t="n">
         <v>326.61</v>
@@ -606,25 +606,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C6" t="n">
-        <v>26.0875613029157</v>
+        <v>26.0857843370626</v>
       </c>
       <c r="D6" t="n">
-        <v>1.650431260855432</v>
+        <v>1.647480850675091</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>25.48</v>
+        <v>25.47</v>
       </c>
       <c r="G6" t="n">
-        <v>26.35</v>
+        <v>26.34</v>
       </c>
       <c r="H6" t="n">
-        <v>27.19</v>
+        <v>27.22</v>
       </c>
       <c r="I6" t="n">
         <v>29.99</v>
@@ -637,13 +637,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C7" t="n">
-        <v>-46.58728803220691</v>
+        <v>-46.57569626279457</v>
       </c>
       <c r="D7" t="n">
-        <v>10.20621201600229</v>
+        <v>10.18534554147162</v>
       </c>
       <c r="E7" t="n">
         <v>-128</v>
@@ -668,13 +668,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8196</v>
+        <v>8401</v>
       </c>
       <c r="C8" t="n">
-        <v>10.26993655441679</v>
+        <v>10.2717771693846</v>
       </c>
       <c r="D8" t="n">
-        <v>1.771792829661422</v>
+        <v>1.772277871327665</v>
       </c>
       <c r="E8" t="n">
         <v>-23.5</v>
@@ -699,13 +699,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C9" t="n">
-        <v>9.386726851287056</v>
+        <v>9.385503451559153</v>
       </c>
       <c r="D9" t="n">
-        <v>1.676426131130018</v>
+        <v>1.676218270986525</v>
       </c>
       <c r="E9" t="n">
         <v>7</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C10" t="n">
-        <v>867.8380261071123</v>
+        <v>867.8385860509402</v>
       </c>
       <c r="D10" t="n">
-        <v>0.46382526644809</v>
+        <v>0.463405568739291</v>
       </c>
       <c r="E10" t="n">
         <v>867.1</v>
@@ -761,28 +761,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8196</v>
+        <v>8401</v>
       </c>
       <c r="C11" t="n">
-        <v>1632.619204489995</v>
+        <v>1656.466492084276</v>
       </c>
       <c r="D11" t="n">
-        <v>1050.750478570848</v>
+        <v>1071.803536369196</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="G11" t="n">
-        <v>1474.5</v>
+        <v>1487</v>
       </c>
       <c r="H11" t="n">
-        <v>2487.25</v>
+        <v>2532</v>
       </c>
       <c r="I11" t="n">
-        <v>3898</v>
+        <v>3966</v>
       </c>
     </row>
     <row r="12">
@@ -792,28 +792,28 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C12" t="n">
-        <v>1743.127729657192</v>
+        <v>1768.274696500833</v>
       </c>
       <c r="D12" t="n">
-        <v>1129.67439147521</v>
+        <v>1151.91236066656</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>801</v>
+        <v>794.25</v>
       </c>
       <c r="G12" t="n">
-        <v>1576</v>
+        <v>1588.5</v>
       </c>
       <c r="H12" t="n">
-        <v>2641</v>
+        <v>2688.75</v>
       </c>
       <c r="I12" t="n">
-        <v>4224</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="13">
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C13" t="n">
-        <v>0.525505163352446</v>
+        <v>0.5251831164008569</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5409177378327277</v>
+        <v>0.5409337532368425</v>
       </c>
       <c r="E13" t="n">
         <v>0.061696</v>
@@ -854,13 +854,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04610345248261561</v>
+        <v>0.04610330873601525</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02173463530691788</v>
+        <v>0.02171281956609874</v>
       </c>
       <c r="E14" t="n">
         <v>0.02</v>
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -947,13 +947,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C17" t="n">
         <v>0.4000000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>5.745754642241973e-14</v>
+        <v>5.829017772356581e-14</v>
       </c>
       <c r="E17" t="n">
         <v>0.4</v>
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C18" t="n">
         <v>3</v>
@@ -1009,13 +1009,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>8197</v>
+        <v>8402</v>
       </c>
       <c r="C19" t="n">
-        <v>62.9872880322069</v>
+        <v>62.97569626279456</v>
       </c>
       <c r="D19" t="n">
-        <v>10.20621201600226</v>
+        <v>10.18534554147152</v>
       </c>
       <c r="E19" t="n">
         <v>44.4</v>

</xml_diff>